<commit_message>
done: update thêm nút RUN ALL + fix output folder cho 3 dạng bài chung "output_audio"
</commit_message>
<xml_diff>
--- a/deploy1.1/backend/uploads/data.xlsx
+++ b/deploy1.1/backend/uploads/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://husteduvn-my.sharepoint.com/personal/cuong_dn210141_sis_hust_edu_vn/Documents/GIT/BÀI-TẬP-IELTS/MiniProd_ContentEngFlow_IELTSStepUpE_T102024/CheckPoint/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://husteduvn-my.sharepoint.com/personal/cuong_dn210141_sis_hust_edu_vn/Documents/GIT/MiniProd_ContentEngFlow_IELTSStepUpE_T102024/deploy1.1/backend/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{741791AC-0435-499B-B3E4-7359D468C0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FBBD4B17-0410-435A-BF78-D865A973C9EE}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{741791AC-0435-499B-B3E4-7359D468C0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8070A438-5F85-4944-A98E-7EA3375578A8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -81,9 +81,6 @@
     <t>MAIN QUESTION</t>
   </si>
   <si>
-    <t>set</t>
-  </si>
-  <si>
     <t>prompt_ipa</t>
   </si>
   <si>
@@ -131,6 +128,9 @@
   </si>
   <si>
     <t>Aubrey and Isaac, engineers, at a construction site</t>
+  </si>
+  <si>
+    <t>set</t>
   </si>
 </sst>
 </file>
@@ -511,25 +511,25 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E8"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="26.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="21.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="34.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="22.28515625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.109375" style="1"/>
+    <col min="3" max="3" width="26.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="34.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="22.33203125" style="1" customWidth="1"/>
     <col min="10" max="10" width="31" style="1" customWidth="1"/>
-    <col min="11" max="12" width="9.140625" style="1"/>
-    <col min="13" max="13" width="60.85546875" style="1" customWidth="1"/>
+    <col min="11" max="12" width="9.109375" style="1"/>
+    <col min="13" max="13" width="60.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -543,7 +543,7 @@
         <v>9</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>6</v>
@@ -555,16 +555,16 @@
         <v>8</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="2" spans="1:16" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -578,25 +578,25 @@
 Situation: Sarah and Tom, neighbors, at a community park</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="K2" s="2" t="str">
         <f>"Topic: "&amp;E2&amp;"
@@ -617,7 +617,7 @@
         <v>curl -L -X POST 'http://103.253.20.13:25010/api/text-to-speech' -H 'Content-Type: application/json' -d '{"text": "Nuclear family","voice": "en-CA-ClaraNeural","speed": 1}' --output 1/ipa.mp3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -631,25 +631,25 @@
 Situation: Aubrey and Isaac, engineers, at a construction site</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="F3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="K3" s="2" t="str">
         <f t="shared" ref="K3" si="1">"Topic: "&amp;E3&amp;"
@@ -670,13 +670,13 @@
         <v>curl -L -X POST 'http://103.253.20.13:25010/api/text-to-speech' -H 'Content-Type: application/json' -d '{"text": "Generational family","voice": "en-CA-ClaraNeural","speed": 1}' --output 2/ipa.mp3</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G5" s="7"/>
     </row>
-    <row r="6" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G6" s="7"/>
     </row>
   </sheetData>

</xml_diff>